<commit_message>
Framework | reader get_dict
</commit_message>
<xml_diff>
--- a/test_data.xlsx
+++ b/test_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Main\Education\QA\GSPOTbackendtest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE104529-155B-479C-9E24-20328D1FE258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1F1D82D-FBAA-4B5F-9023-5517ED91329D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11364" yWindow="1824" windowWidth="11676" windowHeight="10416" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Games" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="256">
   <si>
     <t>name</t>
   </si>
@@ -786,13 +786,65 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>{
+  "name": "string",
+  "developersUuid": "3fa85f64-5717-4562-b3fc-2c963f66afa6",
+  "publishersUuid": "3fa85f64-5717-4562-b3fc-2c963f66afa6",
+  "description": "string",
+  "about": "string",
+  "age": 2147483647,
+  "adult": "string",
+  "type": "GAMES",
+  "systemRequirements": [
+    {
+      "operatingSystem": "LINUX",
+      "deviceProcessor": "string",
+      "deviceMemory": "string",
+      "deviceStorage": "string",
+      "deviceGraphics": "string",
+      "typeRequirements": "MINIMUM"
+    }
+  ],
+  "langs": [
+    {
+      "languageName": "string",
+      "interface": true,
+      "subtitles": true,
+      "voice": true
+    }
+  ],
+  "socials": [
+    {
+      "type": "FACEBOOK",
+      "url": "string"
+    }
+  ],
+  "productOffer": {
+    "offer": {
+      "price": {
+        "amount": "string",
+        "currency": "RUB",
+        "createdBy": "3fa85f64-5717-4562-b3fc-2c963f66afa6",
+        "updatedBy": "3fa85f64-5717-4562-b3fc-2c963f66afa6"
+      },
+      "createdBy": "3fa85f64-5717-4562-b3fc-2c963f66afa6",
+      "isActive": true
+    },
+    "createdBy": "3fa85f64-5717-4562-b3fc-2c963f66afa6"
+  },
+  "genres": [
+    "string"
+  ]
+}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -945,6 +997,15 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -1243,7 +1304,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1286,14 +1347,16 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1327,6 +1390,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1649,13 +1713,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="35.77734375" customWidth="1"/>
+    <col min="3" max="3" width="24.88671875" customWidth="1"/>
     <col min="4" max="4" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1673,7 +1738,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1683,7 +1748,9 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1"/>
+      <c r="D2" s="1" t="s">
+        <v>255</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -1923,7 +1990,7 @@
       <c r="B27" t="s">
         <v>68</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="2" t="s">
         <v>69</v>
       </c>
     </row>
@@ -2636,6 +2703,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C27" r:id="rId1" xr:uid="{6EBAD0EB-483D-47CB-AD4C-2E9154AD0138}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2644,8 +2714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A1:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Framework | change reader
</commit_message>
<xml_diff>
--- a/test_data.xlsx
+++ b/test_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Main\Education\QA\GSPOTbackendtest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1F1D82D-FBAA-4B5F-9023-5517ED91329D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12425BB7-4D4C-43B6-9C14-5E964D6FC1B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11364" yWindow="1824" windowWidth="11676" windowHeight="10416" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Games" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="271">
   <si>
     <t>name</t>
   </si>
@@ -788,63 +788,59 @@
     <t>id</t>
   </si>
   <si>
-    <t>{
-  "name": "string",
-  "developersUuid": "3fa85f64-5717-4562-b3fc-2c963f66afa6",
-  "publishersUuid": "3fa85f64-5717-4562-b3fc-2c963f66afa6",
-  "description": "string",
-  "about": "string",
-  "age": 2147483647,
-  "adult": "string",
-  "type": "GAMES",
-  "systemRequirements": [
-    {
-      "operatingSystem": "LINUX",
-      "deviceProcessor": "string",
-      "deviceMemory": "string",
-      "deviceStorage": "string",
-      "deviceGraphics": "string",
-      "typeRequirements": "MINIMUM"
-    }
-  ],
-  "langs": [
-    {
-      "languageName": "string",
-      "interface": true,
-      "subtitles": true,
-      "voice": true
-    }
-  ],
-  "socials": [
-    {
-      "type": "FACEBOOK",
-      "url": "string"
-    }
-  ],
-  "productOffer": {
-    "offer": {
-      "price": {
-        "amount": "string",
-        "currency": "RUB",
-        "createdBy": "3fa85f64-5717-4562-b3fc-2c963f66afa6",
-        "updatedBy": "3fa85f64-5717-4562-b3fc-2c963f66afa6"
-      },
-      "createdBy": "3fa85f64-5717-4562-b3fc-2c963f66afa6",
-      "isActive": true
-    },
-    "createdBy": "3fa85f64-5717-4562-b3fc-2c963f66afa6"
-  },
-  "genres": [
-    "string"
-  ]
-}</t>
+    <t>https://github.com/victoretc/GSPOTtestingdocumentation/blob/main/games/reference/subgenre/reference_subgenre_list_get.md</t>
+  </si>
+  <si>
+    <t>https://github.com/victoretc/GSPOTtestingdocumentation/blob/main/games/reference/languages/languages_list/laguages_list_positive_get.md</t>
+  </si>
+  <si>
+    <t>https://github.com/victoretc/GSPOTtestingdocumentation/blob/main/games/reference/languages/languages_partial_update/laguages_partial_update_positive_patch.md</t>
+  </si>
+  <si>
+    <t>{"name": ""}</t>
+  </si>
+  <si>
+    <t>{"name": "  "}</t>
+  </si>
+  <si>
+    <t>{"name": "ru "}</t>
+  </si>
+  <si>
+    <t>{"name": " ru"}</t>
+  </si>
+  <si>
+    <t>{"name": "EnGlIsH"}</t>
+  </si>
+  <si>
+    <t>{"name": " qwertyuiopqwertyuiopqwertyuiopqwertyuiopqwertyuiopqwertyuiopqwertyuiopqwertyuiopqwertyuiopqwertyuiopA"}</t>
+  </si>
+  <si>
+    <t>{"name": "qwertyuiopqwertyuiopqwertyuiopqwertyuiopqwertyuiopqwertyuiopqwertyuiopqwertyuiopqwertyuiopqwertyuiop"}</t>
+  </si>
+  <si>
+    <t>{"name": "e"}</t>
+  </si>
+  <si>
+    <t>{"name": "1234567890"}</t>
+  </si>
+  <si>
+    <t>{"name": "Ru En"}</t>
+  </si>
+  <si>
+    <t>{"name": "~!@#$%^&amp;*()_+&lt;&gt;?:/|{}[]';,.`-="}</t>
+  </si>
+  <si>
+    <t>{"name": "Հայկականتحتاجفقطإلىنسخלבדוק"}</t>
+  </si>
+  <si>
+    <t>{"name": "下来顔文字"}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1005,6 +1001,11 @@
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF6A8759"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1349,12 +1350,15 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1711,20 +1715,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D105"/>
+  <dimension ref="A1:E105"/>
   <sheetViews>
-    <sheetView topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="G85" sqref="G85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="35.77734375" customWidth="1"/>
-    <col min="3" max="3" width="24.88671875" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" customWidth="1"/>
+    <col min="2" max="2" width="46.44140625" customWidth="1"/>
+    <col min="3" max="3" width="22.44140625" customWidth="1"/>
+    <col min="4" max="4" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>254</v>
       </c>
@@ -1738,7 +1742,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1748,11 +1752,9 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1763,7 +1765,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1771,7 +1773,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1779,7 +1781,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1787,7 +1789,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1795,7 +1797,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1803,7 +1805,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1811,7 +1813,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1822,7 +1824,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -1833,7 +1835,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -1844,7 +1846,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -1855,7 +1857,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -1866,7 +1868,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -1877,7 +1879,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>39</v>
       </c>
@@ -1888,7 +1890,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>42</v>
       </c>
@@ -1899,7 +1901,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -1910,7 +1912,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>48</v>
       </c>
@@ -1921,7 +1923,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>51</v>
       </c>
@@ -1932,7 +1934,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>54</v>
       </c>
@@ -1943,7 +1945,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>57</v>
       </c>
@@ -1951,7 +1953,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>59</v>
       </c>
@@ -1959,7 +1961,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>61</v>
       </c>
@@ -1967,7 +1969,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>63</v>
       </c>
@@ -1975,7 +1977,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>65</v>
       </c>
@@ -1983,7 +1985,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
         <v>67</v>
       </c>
@@ -1994,7 +1996,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
         <v>70</v>
       </c>
@@ -2002,7 +2004,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
         <v>72</v>
       </c>
@@ -2010,7 +2012,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3">
       <c r="A30" t="s">
         <v>74</v>
       </c>
@@ -2018,7 +2020,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3">
       <c r="A31" t="s">
         <v>76</v>
       </c>
@@ -2026,7 +2028,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3">
       <c r="A32" t="s">
         <v>78</v>
       </c>
@@ -2034,7 +2036,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3">
       <c r="A33" t="s">
         <v>80</v>
       </c>
@@ -2042,7 +2044,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3">
       <c r="A34" t="s">
         <v>82</v>
       </c>
@@ -2050,7 +2052,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3">
       <c r="A35" t="s">
         <v>84</v>
       </c>
@@ -2058,7 +2060,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3">
       <c r="A36" t="s">
         <v>86</v>
       </c>
@@ -2066,7 +2068,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3">
       <c r="A37" t="s">
         <v>88</v>
       </c>
@@ -2074,7 +2076,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3">
       <c r="A38" t="s">
         <v>90</v>
       </c>
@@ -2082,7 +2084,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3">
       <c r="A39" t="s">
         <v>92</v>
       </c>
@@ -2090,7 +2092,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3">
       <c r="A40" t="s">
         <v>94</v>
       </c>
@@ -2101,7 +2103,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3">
       <c r="A41" t="s">
         <v>97</v>
       </c>
@@ -2109,7 +2111,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3">
       <c r="A42" t="s">
         <v>99</v>
       </c>
@@ -2117,7 +2119,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3">
       <c r="A43" t="s">
         <v>101</v>
       </c>
@@ -2125,7 +2127,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3">
       <c r="A44" t="s">
         <v>103</v>
       </c>
@@ -2133,7 +2135,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3">
       <c r="A45" t="s">
         <v>105</v>
       </c>
@@ -2141,7 +2143,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3">
       <c r="A46" t="s">
         <v>107</v>
       </c>
@@ -2149,7 +2151,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3">
       <c r="A47" t="s">
         <v>109</v>
       </c>
@@ -2157,7 +2159,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3">
       <c r="A48" t="s">
         <v>111</v>
       </c>
@@ -2165,7 +2167,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3">
       <c r="A49" t="s">
         <v>113</v>
       </c>
@@ -2173,7 +2175,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3">
       <c r="A50" t="s">
         <v>115</v>
       </c>
@@ -2184,7 +2186,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3">
       <c r="A51" t="s">
         <v>118</v>
       </c>
@@ -2192,7 +2194,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3">
       <c r="A52" t="s">
         <v>120</v>
       </c>
@@ -2200,7 +2202,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3">
       <c r="A53" t="s">
         <v>122</v>
       </c>
@@ -2208,7 +2210,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3">
       <c r="A54" t="s">
         <v>124</v>
       </c>
@@ -2216,7 +2218,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3">
       <c r="A55" t="s">
         <v>126</v>
       </c>
@@ -2224,7 +2226,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3">
       <c r="A56" t="s">
         <v>128</v>
       </c>
@@ -2232,7 +2234,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3">
       <c r="A57" t="s">
         <v>130</v>
       </c>
@@ -2240,7 +2242,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3">
       <c r="A58" t="s">
         <v>132</v>
       </c>
@@ -2248,7 +2250,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3">
       <c r="A59" t="s">
         <v>134</v>
       </c>
@@ -2256,7 +2258,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3">
       <c r="A60" t="s">
         <v>136</v>
       </c>
@@ -2264,7 +2266,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3">
       <c r="A61" t="s">
         <v>138</v>
       </c>
@@ -2272,7 +2274,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3">
       <c r="A62" t="s">
         <v>140</v>
       </c>
@@ -2280,7 +2282,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3">
       <c r="A63" t="s">
         <v>142</v>
       </c>
@@ -2288,7 +2290,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3">
       <c r="A64" t="s">
         <v>144</v>
       </c>
@@ -2296,7 +2298,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4">
       <c r="A65" t="s">
         <v>146</v>
       </c>
@@ -2304,7 +2306,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4">
       <c r="A66" t="s">
         <v>148</v>
       </c>
@@ -2312,7 +2314,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4">
       <c r="A67" t="s">
         <v>150</v>
       </c>
@@ -2320,7 +2322,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4">
       <c r="A68" t="s">
         <v>152</v>
       </c>
@@ -2328,7 +2330,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4">
       <c r="A69" t="s">
         <v>154</v>
       </c>
@@ -2336,7 +2338,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4">
       <c r="A70" t="s">
         <v>156</v>
       </c>
@@ -2344,7 +2346,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4">
       <c r="A71" t="s">
         <v>158</v>
       </c>
@@ -2352,7 +2354,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4">
       <c r="A72" t="s">
         <v>160</v>
       </c>
@@ -2360,7 +2362,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4">
       <c r="A73" t="s">
         <v>162</v>
       </c>
@@ -2368,7 +2370,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4">
       <c r="A74" t="s">
         <v>164</v>
       </c>
@@ -2376,7 +2378,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4">
       <c r="A75" t="s">
         <v>166</v>
       </c>
@@ -2387,7 +2389,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4">
       <c r="A76" t="s">
         <v>169</v>
       </c>
@@ -2395,7 +2397,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" ht="72">
       <c r="A77" t="s">
         <v>171</v>
       </c>
@@ -2405,8 +2407,11 @@
       <c r="C77" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D77" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="72">
       <c r="A78" t="s">
         <v>174</v>
       </c>
@@ -2416,8 +2421,11 @@
       <c r="C78" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D78" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
       <c r="A79" t="s">
         <v>177</v>
       </c>
@@ -2427,8 +2435,11 @@
       <c r="C79" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D79" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
       <c r="A80" t="s">
         <v>180</v>
       </c>
@@ -2438,8 +2449,11 @@
       <c r="C80" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D80" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
       <c r="A81" t="s">
         <v>183</v>
       </c>
@@ -2447,7 +2461,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5">
       <c r="A82" t="s">
         <v>185</v>
       </c>
@@ -2457,8 +2471,12 @@
       <c r="C82" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D82" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="E82" s="3"/>
+    </row>
+    <row r="83" spans="1:5">
       <c r="A83" t="s">
         <v>188</v>
       </c>
@@ -2468,8 +2486,11 @@
       <c r="C83" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D83" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
       <c r="A84" t="s">
         <v>191</v>
       </c>
@@ -2479,19 +2500,25 @@
       <c r="C84" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D84" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="43.2">
       <c r="A85" t="s">
         <v>194</v>
       </c>
       <c r="B85" t="s">
         <v>195</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C85" s="2" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D85" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
       <c r="A86" t="s">
         <v>197</v>
       </c>
@@ -2501,8 +2528,11 @@
       <c r="C86" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D86" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
       <c r="A87" t="s">
         <v>200</v>
       </c>
@@ -2512,8 +2542,12 @@
       <c r="C87" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D87" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E87" s="3"/>
+    </row>
+    <row r="88" spans="1:5">
       <c r="A88" t="s">
         <v>203</v>
       </c>
@@ -2523,8 +2557,11 @@
       <c r="C88" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D88" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="43.2">
       <c r="A89" t="s">
         <v>206</v>
       </c>
@@ -2534,8 +2571,11 @@
       <c r="C89" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D89" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
       <c r="A90" t="s">
         <v>209</v>
       </c>
@@ -2545,8 +2585,11 @@
       <c r="C90" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D90" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
       <c r="A91" t="s">
         <v>212</v>
       </c>
@@ -2557,7 +2600,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5">
       <c r="A92" t="s">
         <v>215</v>
       </c>
@@ -2568,7 +2611,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5">
       <c r="A93" t="s">
         <v>218</v>
       </c>
@@ -2579,23 +2622,29 @@
         <v>220</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5">
       <c r="A94" t="s">
         <v>221</v>
       </c>
       <c r="B94" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C94" s="2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
       <c r="A95" t="s">
         <v>223</v>
       </c>
       <c r="B95" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C95" s="2" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
       <c r="A96" t="s">
         <v>225</v>
       </c>
@@ -2606,7 +2655,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4">
       <c r="A97" t="s">
         <v>228</v>
       </c>
@@ -2617,7 +2666,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4">
       <c r="A98" t="s">
         <v>231</v>
       </c>
@@ -2628,18 +2677,21 @@
         <v>233</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4">
       <c r="A99" t="s">
         <v>234</v>
       </c>
       <c r="B99" t="s">
         <v>235</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C99" s="2" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D99" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
       <c r="A100" t="s">
         <v>237</v>
       </c>
@@ -2649,27 +2701,33 @@
       <c r="C100" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D100" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
       <c r="A101" t="s">
         <v>240</v>
       </c>
       <c r="B101" t="s">
         <v>241</v>
       </c>
-      <c r="C101" t="s">
+      <c r="C101" s="2" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4">
       <c r="A102" t="s">
         <v>243</v>
       </c>
       <c r="B102" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C102" s="2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
       <c r="A103" t="s">
         <v>245</v>
       </c>
@@ -2680,7 +2738,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4">
       <c r="A104" t="s">
         <v>248</v>
       </c>
@@ -2691,7 +2749,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4">
       <c r="A105" t="s">
         <v>251</v>
       </c>
@@ -2705,8 +2763,15 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C27" r:id="rId1" xr:uid="{6EBAD0EB-483D-47CB-AD4C-2E9154AD0138}"/>
+    <hyperlink ref="C102" r:id="rId2" xr:uid="{7E6AE852-CC07-4B70-9A50-71E4474BF080}"/>
+    <hyperlink ref="C94" r:id="rId3" xr:uid="{7B5B54F2-214A-4956-BF5B-D0231A591AEC}"/>
+    <hyperlink ref="C95" r:id="rId4" xr:uid="{E820759A-9698-499E-88FC-09DF1D90BA93}"/>
+    <hyperlink ref="C101" r:id="rId5" xr:uid="{56B166C5-B112-4763-9016-A152DA466F4D}"/>
+    <hyperlink ref="C99" r:id="rId6" xr:uid="{7FBDCA6B-153F-4BAD-AADE-7298D6880100}"/>
+    <hyperlink ref="C85" r:id="rId7" xr:uid="{4A0C09A3-3851-4881-BFFF-11EEC229AFC7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -2714,13 +2779,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A1:A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="2" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="4:4">
       <c r="D2" s="1"/>
     </row>
   </sheetData>

</xml_diff>